<commit_message>
added definitions of naturalness
</commit_message>
<xml_diff>
--- a/Opinion_paper/OSF/Literature_overview_72_publications.xlsx
+++ b/Opinion_paper/OSF/Literature_overview_72_publications.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20411"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AA7A18-503B-41B9-927A-E173CF53F6E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15816BF2-CFF3-4657-A882-1DAC11489867}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>Systematic review</t>
   </si>
   <si>
-    <t>“Speech is natural if it conforms to the listener’s standard of rate, rhythm, intonation, and stress patterning, and if it conforms to the syntactic structure of the utterance being produced” (Yorkston, Beukelman, Strand, &amp; Bell, 1999, p. 464).</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Rodero, E., &amp; Lucas, I. (2023). Synthetic versus human voices in audiobooks: The human emotional intimacy effect. </t>
     </r>
@@ -793,9 +790,6 @@
     </r>
   </si>
   <si>
-    <t>"Natural speech was defined for this study as conventional in terms of intonation, voice quality, rate, rhythm, or intensity adjustments. Unnatural or bizarre speech, on the other hand, was defined as markedly deviating from the expected or conventional pattern."</t>
-  </si>
-  <si>
     <t>dysarthria affects naturalness, linked with speech rate, but only in normal speakers, because dysathria was already so unnatural that it did not make a difference</t>
   </si>
   <si>
@@ -847,9 +841,6 @@
   </si>
   <si>
     <t>Vowels produced with jitter+shimmer were considered as the most natural. Vowels with shimmer and without perturbation were considered as the most artificial</t>
-  </si>
-  <si>
-    <t>"Naturalness refers to how closely the output sounds like human speech"</t>
   </si>
   <si>
     <t>Tamagawa, R., Watson, C. I., Kuo, I. H., MacDonald, B. A., &amp; Broadbent, E. (2011). The effects of synthesized voice accents on user perceptions of robots. International Journal of Social Robotics, 3, 253-262.</t>
@@ -2259,10 +2250,6 @@
 speakers. Speakers rated as less natural took longer to identify and were identified less accurately in the gender identification task; and  rated as less prototypically masculine/feminine"</t>
   </si>
   <si>
-    <t>"speech naturalness has been conceptualized as a listener’s scaling between an individual’s speech and
-the listener’s representation of typical speech patterns, including the dimensions of rate, rhythm, intonation, stress patterning, and syntactic structure" (p.1)</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Klopfenstein, M. (2016). Speech naturalness ratings and perceptual correlates of highly natural and unnatural speech in hypokinetic dysarthria secondary to Parkinson's disease. </t>
     </r>
@@ -2936,15 +2923,7 @@
     <t>performance data</t>
   </si>
   <si>
-    <t>"naturalness was defined as conforming to “the listener’s standards of rate, rhythm, intonation, and stress patterning” and to “the syntactic structure of the utterance
-being produced” (Yorkston 2010, p228), p 4687</t>
-  </si>
-  <si>
     <t>Deviation-based</t>
-  </si>
-  <si>
-    <t>"Speech naturalness can be described as how the speech of a person with a speech disorder compares with that of typical
-speech or, in the case of an acquired disorder, how an individual’s speech compares to its premorbid state" (p 1)</t>
   </si>
   <si>
     <t>human-manipulated</t>
@@ -2968,10 +2947,6 @@
     <t>human-likeness, anthropomorphism, artificiality</t>
   </si>
   <si>
-    <t>"Human likeness has been used, […] to describe how accurately the machine
-is able to imitate a human" (p. 2)</t>
-  </si>
-  <si>
     <t>Both</t>
   </si>
   <si>
@@ -2990,11 +2965,6 @@
     <t>human-healthy</t>
   </si>
   <si>
-    <t>"Speech Naturalness is a term defined from the
-listener's perspective as speech that "sounds normal or natural" and allows
-the listener's attention to focus on the message rather than the speech pattern" (page 1)</t>
-  </si>
-  <si>
     <t>disfluency</t>
   </si>
   <si>
@@ -3007,17 +2977,7 @@
     <t>rating data + ERPs</t>
   </si>
   <si>
-    <t>naturalness - "acoustic tendencies that define naturalness from human to synthesized
-voices." (p1); "neural specialization of the human brain to process speech is
-underlined by acoustic properties that are perceived as voice naturalness (i.e., speech intrinsic property to be recognized as
-a social ecological sound)." (p2)</t>
-  </si>
-  <si>
     <t>human voice consistency, naturalistic quality</t>
-  </si>
-  <si>
-    <t>“a perceptually derived,
-overall description of prosodic adequacy.” (p4)  + Yorkston definition</t>
   </si>
   <si>
     <t>acceptability, severity</t>
@@ -3040,10 +3000,6 @@
     <t>realism, human-likeness, anthropomorphism</t>
   </si>
   <si>
-    <t>"‘‘Humanoid’’ is adopted as the working term in this article to refer to the state of being humanlike but bearing
-the clear artificiality of computer synthesis." (page 2)</t>
-  </si>
-  <si>
     <t>self-disclosure in interview</t>
   </si>
   <si>
@@ -3051,9 +3007,6 @@
   </si>
   <si>
     <t>realism, human-likeness, robotic, anthropomorphism, expressiveness</t>
-  </si>
-  <si>
-    <t>dual humanness (speaking and listening), "Humanness perception of technology is defined as the degree to which a user feels a certain technology or system is human-like (versus machine-like)" (p 3)</t>
   </si>
   <si>
     <t>rating data + EMG</t>
@@ -3078,17 +3031,9 @@
     <t>accentedness</t>
   </si>
   <si>
-    <t>"Speech is natural if it conforms to the listener’s standard of rate, rhythm, intonation and stress patterning, and if it conforms to the syntactic structure of the utterance being produced" (p 2)</t>
-  </si>
-  <si>
     <t>impairment, severity</t>
   </si>
   <si>
-    <t>"Naturalness’ will not be defined for you." (p7) "sounding ‘natural’ may
-be speaking like she or he did before the onset of dysarthria, even if such a
-goal is out of reach" (p 2)</t>
-  </si>
-  <si>
     <t>systematic review</t>
   </si>
   <si>
@@ -3105,10 +3050,6 @@
   </si>
   <si>
     <t>rating data, fNIRS, eye tracking</t>
-  </si>
-  <si>
-    <t>"Among the factors, anthropomorphism,
-which is the assignment of a human form, characteristics, orbehavior to nonhuman objects, emerges as a decisive force " (p 1)</t>
   </si>
   <si>
     <t>realism</t>
@@ -3125,19 +3066,12 @@
     <t>normalcy</t>
   </si>
   <si>
-    <t>"naturalness will not be defined for you"</t>
-  </si>
-  <si>
     <t>"‘‘natural speech’’ is the speech most closely perceived as a human voice" (p 10)</t>
   </si>
   <si>
     <t>quality, appropriateness</t>
   </si>
   <si>
-    <t>"that is, with regard to how much like real
-speech each utterance seemed to be" (p 6)</t>
-  </si>
-  <si>
     <t>voice-appearance matching task</t>
   </si>
   <si>
@@ -3153,11 +3087,6 @@
     <t>voice quality, acceptability</t>
   </si>
   <si>
-    <t>"There is no extant objective definition of naturalness
-that we are aware of--it is a voice quality that is purely
-subjective." (p. 2)</t>
-  </si>
-  <si>
     <t>two-alternative forced choice task</t>
   </si>
   <si>
@@ -3173,9 +3102,6 @@
     <t>normal, acceptability, speech quality</t>
   </si>
   <si>
-    <t>"naturalness is the quality by which a voice sounds more similar to human speech" (p 1)</t>
-  </si>
-  <si>
     <t>artificial, prosody quality</t>
   </si>
   <si>
@@ -3195,13 +3121,6 @@
   </si>
   <si>
     <t>dysarthria, severity</t>
-  </si>
-  <si>
-    <t>conversational naturalness: "an interaction that has the same conversational flow as humans have interacting with each other" (p 2)</t>
-  </si>
-  <si>
-    <t>"degree to which individuals sound ‘different’ from
-healthy peers" (p 6)</t>
   </si>
   <si>
     <t>sorting method</t>
@@ -3727,23 +3646,102 @@
     <t>Study ID</t>
   </si>
   <si>
+    <t xml:space="preserve">Conceptuaization: Human-Likeness; Deviation-based; Both </t>
+  </si>
+  <si>
+    <t>dysprosody, monopitch, bizarreness, acceptability</t>
+  </si>
+  <si>
+    <t>anthropomorphism; realism</t>
+  </si>
+  <si>
+    <t>artificial voices</t>
+  </si>
+  <si>
+    <t>tracheoesophageal speech; perceptual scaling; alaryngeal speech; naturalness; severity</t>
+  </si>
+  <si>
+    <t>"[..] acoustic tendencies that define naturalness from human to synthesized
+voices." (p1); "neural specialization of the human brain to process speech is
+underlined by acoustic properties that are perceived as voice naturalness (i.e., speech intrinsic property to be recognized as
+a social ecological sound)." (p2)</t>
+  </si>
+  <si>
     <t>"Speech naturalness has
-been defined as speech output that sounds normal or natural to the listener (Parrish, 1951)." (p2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conceptuaization: Human-Likeness; Deviation-based; Both </t>
-  </si>
-  <si>
-    <t>dysprosody, monopitch, bizarreness, acceptability</t>
-  </si>
-  <si>
-    <t>anthropomorphism; realism</t>
-  </si>
-  <si>
-    <t>artificial voices</t>
-  </si>
-  <si>
-    <t>tracheoesophageal speech; perceptual scaling; alaryngeal speech; naturalness; severity</t>
+been defined as speech output that sounds normal or natural to the listener (Parrish, 1951)." (p11)</t>
+  </si>
+  <si>
+    <t>"naturalness was defined as conforming to “the listener’s standards of rate, rhythm, intonation, and stress patterning” and to “the syntactic structure of the utterance
+being produced” (p 4687)</t>
+  </si>
+  <si>
+    <t>"Speech naturalness can be described as how the speech of a person with a speech disorder compares with that of typical
+speech or, in the case of an acquired disorder, how an individual’s speech compares to its premorbid state" (p 1134)</t>
+  </si>
+  <si>
+    <t>"Speech Naturalness is a term defined from the
+listener's perspective as speech that "sounds normal or natural" and allows
+the listener's attention to focus on the message rather than the speech pattern" (page 295)</t>
+  </si>
+  <si>
+    <t>“Naturalness was defined as a perceptually derived, overall description of prosodic adequacy. That is, speech was defined as natural if it conforms to the listener’s standards of rate, rhythm, intonation, and stress pattern, and if it conforms to the syntactic structure of the utterance being produced” (page 1091)</t>
+  </si>
+  <si>
+    <t>"Speech is natural if it conforms to the listener’s standard of rate, rhythm, intonation and stress patterning, and if it conforms to the syntactic structure of the utterance being produced" (p 938)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "sounding ‘natural’ may
+be speaking like she or he did before the onset of dysarthria, even if such a
+goal is out of reach" (p 124)</t>
+  </si>
+  <si>
+    <t>“Speech is natural if it conforms to the listener’s standard of rate, rhythm, intonation, and stress patterning, and if it conforms to the syntactic structure of the utterance being produced”  (p. 327).</t>
+  </si>
+  <si>
+    <t>"naturalness will not be defined for you" (page 54)</t>
+  </si>
+  <si>
+    <t>"speech naturalness has been conceptualized as a listener’s scaling between an individual’s speech and
+the listener’s representation of typical speech patterns, including the dimensions of rate, rhythm, intonation, stress patterning, and syntactic structure" (p.2054)</t>
+  </si>
+  <si>
+    <t>"degree to which individuals sound ‘different’ from
+healthy peers" (p 1265)</t>
+  </si>
+  <si>
+    <t>"Natural speech was defined for this study as conventional in terms of intonation, voice quality, rate, rhythm, or intensity adjustments. Unnatural or bizarre speech, on the other hand, was defined as markedly deviating from the expected or conventional pattern." (page 551)</t>
+  </si>
+  <si>
+    <t>"Human likeness has been used, […] to describe how accurately the machine
+is able to imitate a human" (p. 2864)</t>
+  </si>
+  <si>
+    <t>"‘‘Humanoid’’ is adopted as the working term in this article to refer to the state of being humanlike but bearing
+the clear artificiality of computer synthesis." (page 164)</t>
+  </si>
+  <si>
+    <t>"Humanness perception of technology is defined as the degree to which a user feels a certain technology or system is human-like (versus machine-like)" (p 3)</t>
+  </si>
+  <si>
+    <t>“anthropomorphism, which is the assignment of a human form, characteristics, or behavior to nonhuman objects […].” (page 1)</t>
+  </si>
+  <si>
+    <t>"that is, with regard to how much like real
+speech each utterance seemed to be" (p 316)</t>
+  </si>
+  <si>
+    <t>"There is no extant objective definition of naturalness
+that we are aware of--it is a voice quality that is purely
+subjective." (p. 8)</t>
+  </si>
+  <si>
+    <t>"naturalness is the quality by which a voice sounds more similar to human speech" (p 336)</t>
+  </si>
+  <si>
+    <t>conversational naturalness: "an interaction that has the same conversational flow as humans have interacting with each other" (p 570)</t>
+  </si>
+  <si>
+    <t>"Naturalness refers to how closely the output sounds like human speech" 8page 389.e1)</t>
   </si>
 </sst>
 </file>
@@ -4254,10 +4252,10 @@
   <dimension ref="A1:AX73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B71" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B79" sqref="B79"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4281,13 +4279,13 @@
   <sheetData>
     <row r="1" spans="1:50" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>522</v>
+        <v>501</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>521</v>
+        <v>500</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>1</v>
@@ -4299,113 +4297,113 @@
         <v>2</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>457</v>
+        <v>436</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>524</v>
+        <v>502</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="M1" s="12" t="s">
         <v>3</v>
       </c>
       <c r="N1" s="14" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="O1" s="14" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2" spans="1:50" s="16" customFormat="1" ht="204" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D2" s="16">
         <v>2022</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="N2" s="16" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:50" s="29" customFormat="1" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D3" s="29">
         <v>2021</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>365</v>
+        <v>509</v>
       </c>
       <c r="I3" s="35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K3" s="36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L3" s="29" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="M3" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
@@ -4447,255 +4445,255 @@
     </row>
     <row r="4" spans="1:50" s="3" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D4" s="29">
         <v>2015</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>510</v>
+      </c>
+      <c r="I4" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="29" t="s">
+        <v>361</v>
+      </c>
+      <c r="K4" s="29" t="s">
+        <v>503</v>
+      </c>
+      <c r="L4" s="29" t="s">
+        <v>358</v>
+      </c>
+      <c r="M4" s="29" t="s">
         <v>19</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>363</v>
-      </c>
-      <c r="H4" s="29" t="s">
-        <v>367</v>
-      </c>
-      <c r="I4" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="29" t="s">
-        <v>366</v>
-      </c>
-      <c r="K4" s="29" t="s">
-        <v>525</v>
-      </c>
-      <c r="L4" s="29" t="s">
-        <v>362</v>
-      </c>
-      <c r="M4" s="29" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:50" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D5" s="3">
         <v>2006</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="29" t="s">
+        <v>361</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="I5" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="29" t="s">
-        <v>366</v>
-      </c>
-      <c r="K5" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:50" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D6" s="16">
         <v>2017</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N6" s="16" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="7" spans="1:50" s="16" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D7" s="16">
         <v>2017</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N7" s="18" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:50" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D8" s="16">
         <v>2018</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>374</v>
+        <v>520</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M8" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N8" s="16" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:50" s="19" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D9" s="16">
         <v>2018</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M9" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N9" s="18"/>
       <c r="O9" s="16"/>
@@ -4737,126 +4735,126 @@
     </row>
     <row r="10" spans="1:50" s="4" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D10" s="4">
         <v>2017</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:50" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D11" s="4">
         <v>2021</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="12" spans="1:50" s="19" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D12" s="16">
         <v>2017</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M12" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N12" s="16" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="O12" s="16"/>
       <c r="P12" s="16"/>
@@ -4897,132 +4895,132 @@
     </row>
     <row r="13" spans="1:50" s="3" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D13" s="3">
         <v>2005</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="I13" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="I13" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:50" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>508</v>
+        <v>487</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>509</v>
+        <v>488</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D14" s="4">
         <v>2024</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>453</v>
+        <v>432</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="N14" s="38" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="O14" s="6"/>
     </row>
-    <row r="15" spans="1:50" s="4" customFormat="1" ht="225" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" s="4" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D15" s="4">
         <v>2022</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>386</v>
+        <v>507</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
@@ -5062,303 +5060,303 @@
     </row>
     <row r="16" spans="1:50" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>466</v>
+        <v>445</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>467</v>
+        <v>446</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D16" s="4">
         <v>2024</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>461</v>
+        <v>440</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>510</v>
+        <v>489</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>468</v>
+        <v>447</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>469</v>
+        <v>448</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>470</v>
+        <v>449</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:50" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:50" s="3" customFormat="1" ht="195" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D17" s="3">
         <v>2002</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="G17" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>388</v>
+        <v>512</v>
       </c>
       <c r="I17" s="26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>454</v>
+        <v>433</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>528</v>
+        <v>506</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:50" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D18" s="3">
         <v>2008</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="G18" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="I18" s="26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="19" spans="1:50" s="4" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D19" s="6">
         <v>2021</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="1:50" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D20" s="3">
         <v>2021</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="I20" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K20" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="21" spans="1:50" s="16" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D21" s="16">
         <v>2012</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="L21" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M21" s="16" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="N21" s="18" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="O21" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:50" s="16" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D22" s="19">
         <v>2021</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="H22" s="19"/>
       <c r="I22" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J22" s="19" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K22" s="19" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="L22" s="19" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M22" s="19" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="N22" s="18" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="O22" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P22" s="19"/>
       <c r="Q22" s="19"/>
@@ -5398,585 +5396,585 @@
     </row>
     <row r="23" spans="1:50" s="16" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D23" s="16">
         <v>2007</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>395</v>
+        <v>521</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K23" s="16" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="L23" s="16" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
       <c r="M23" s="16" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:50" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D24" s="3">
         <v>2016</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>511</v>
+        <v>490</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="I24" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:50" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D25" s="3">
         <v>2020</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="I25" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K25" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:50" s="16" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D26" s="16">
         <v>2022</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="I26" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K26" s="16" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
       <c r="L26" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M26" s="16" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N26" s="16" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
-    <row r="27" spans="1:50" s="16" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:50" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D27" s="16">
         <v>2021</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F27" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>356</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>522</v>
+      </c>
+      <c r="I27" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J27" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="K27" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="G27" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>399</v>
-      </c>
-      <c r="I27" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="J27" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="K27" s="16" t="s">
-        <v>46</v>
-      </c>
       <c r="L27" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M27" s="16" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="N27" s="18" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="O27" s="16" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="28" spans="1:50" s="16" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>471</v>
+        <v>450</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>472</v>
+        <v>451</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>473</v>
+        <v>452</v>
       </c>
       <c r="D28" s="16">
         <v>2024</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>475</v>
+        <v>454</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>474</v>
+        <v>453</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>477</v>
+        <v>456</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J28" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K28" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L28" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M28" s="16" t="s">
-        <v>478</v>
+        <v>457</v>
       </c>
       <c r="N28" s="16" t="s">
-        <v>476</v>
+        <v>455</v>
       </c>
       <c r="O28" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:50" s="4" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D29" s="4">
         <v>2011</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="O29" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:50" s="16" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D30" s="16">
         <v>2013</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J30" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K30" s="16" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
       <c r="L30" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M30" s="16" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N30" s="16" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="O30" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:50" s="16" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D31" s="16">
         <v>2023</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
       <c r="I31" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J31" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K31" s="16" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
       <c r="L31" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M31" s="16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="N31" s="18" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="32" spans="1:50" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
-        <v>479</v>
+        <v>458</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>480</v>
+        <v>459</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>481</v>
+        <v>460</v>
       </c>
       <c r="D32" s="3">
         <v>2019</v>
       </c>
       <c r="E32" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="I32" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="K32" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>512</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>483</v>
-      </c>
-      <c r="I32" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="K32" s="3" t="s">
-        <v>482</v>
-      </c>
       <c r="L32" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>484</v>
+        <v>463</v>
       </c>
       <c r="N32" s="3" t="s">
-        <v>485</v>
+        <v>464</v>
       </c>
     </row>
     <row r="33" spans="1:15" s="4" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D33" s="4">
         <v>2022</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>513</v>
+        <v>492</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="34" spans="1:15" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D34" s="3">
         <v>2015</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>407</v>
+        <v>513</v>
       </c>
       <c r="I34" s="26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>408</v>
+        <v>395</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="35" spans="1:15" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D35" s="3">
         <v>2016</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>409</v>
+        <v>514</v>
       </c>
       <c r="I35" s="26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>455</v>
+        <v>434</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="N35" s="3" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="O35" s="3" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B36" s="29" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D36" s="29">
         <v>2020</v>
@@ -5985,816 +5983,816 @@
         <v>6</v>
       </c>
       <c r="F36" s="29" t="s">
-        <v>514</v>
+        <v>493</v>
       </c>
       <c r="G36" s="29" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="H36" s="29" t="s">
-        <v>7</v>
+        <v>515</v>
       </c>
       <c r="I36" s="35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J36" s="29" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K36" s="29" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="L36" s="29" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="M36" s="29"/>
       <c r="N36" s="3" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="37" spans="1:15" s="16" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D37" s="16">
         <v>2023</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>515</v>
+        <v>494</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="I37" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J37" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K37" s="16" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="L37" s="16" t="s">
-        <v>456</v>
+        <v>435</v>
       </c>
       <c r="M37" s="16" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="N37" s="16" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="38" spans="1:15" s="16" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D38" s="16">
         <v>2020</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F38" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="I38" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J38" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K38" s="16" t="s">
-        <v>451</v>
+        <v>430</v>
       </c>
       <c r="L38" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M38" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N38" s="18" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="39" spans="1:15" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D39" s="16">
         <v>2010</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F39" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G39" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="I39" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J39" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K39" s="16" t="s">
-        <v>448</v>
+        <v>427</v>
       </c>
       <c r="L39" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M39" s="16" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="N39" s="16" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="O39" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:15" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
-        <v>494</v>
+        <v>473</v>
       </c>
       <c r="B40" s="34" t="s">
-        <v>495</v>
+        <v>474</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>496</v>
+        <v>475</v>
       </c>
       <c r="D40" s="3">
         <v>2022</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>461</v>
+        <v>440</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>497</v>
+        <v>476</v>
       </c>
       <c r="I40" s="26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>498</v>
+        <v>477</v>
       </c>
       <c r="N40" s="3" t="s">
-        <v>499</v>
+        <v>478</v>
       </c>
     </row>
     <row r="41" spans="1:15" s="16" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D41" s="16">
         <v>2023</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G41" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="H41" s="16" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
       <c r="I41" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J41" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K41" s="16" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
       <c r="L41" s="16" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
       <c r="M41" s="16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="N41" s="18" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="O41" s="16" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
-    <row r="42" spans="1:15" s="16" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D42" s="16">
         <v>2021</v>
       </c>
       <c r="E42" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F42" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="H42" s="16" t="s">
+        <v>523</v>
+      </c>
+      <c r="I42" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J42" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="K42" s="16" t="s">
+        <v>399</v>
+      </c>
+      <c r="L42" s="16" t="s">
+        <v>358</v>
+      </c>
+      <c r="M42" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G42" s="16" t="s">
-        <v>368</v>
-      </c>
-      <c r="H42" s="16" t="s">
-        <v>416</v>
-      </c>
-      <c r="I42" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="J42" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="K42" s="16" t="s">
-        <v>413</v>
-      </c>
-      <c r="L42" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="M42" s="16" t="s">
-        <v>17</v>
-      </c>
       <c r="N42" s="16" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="O42" s="16" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="43" spans="1:15" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D43" s="3">
         <v>1997</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>516</v>
+        <v>495</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="I43" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>452</v>
+        <v>431</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N43" s="3" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="44" spans="1:15" s="4" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D44" s="4">
         <v>2019</v>
       </c>
       <c r="E44" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="L44" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="M44" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F44" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>360</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>418</v>
-      </c>
-      <c r="I44" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>375</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="L44" s="4" t="s">
-        <v>419</v>
-      </c>
-      <c r="M44" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="N44" s="4" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="45" spans="1:15" s="3" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A45" s="24" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D45" s="3">
         <v>1984</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>421</v>
+        <v>516</v>
       </c>
       <c r="I45" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:15" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D46" s="16">
         <v>2022</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>517</v>
+        <v>496</v>
       </c>
       <c r="G46" s="16" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="H46" s="16" t="s">
-        <v>422</v>
+        <v>406</v>
       </c>
       <c r="I46" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J46" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K46" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L46" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M46" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="N46" s="16" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="47" spans="1:15" s="16" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D47" s="16">
         <v>2011</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F47" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G47" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>424</v>
+        <v>524</v>
       </c>
       <c r="I47" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J47" s="19" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K47" s="16" t="s">
-        <v>423</v>
+        <v>407</v>
       </c>
       <c r="L47" s="16" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="M47" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N47" s="16" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="O47" s="19"/>
     </row>
     <row r="48" spans="1:15" s="16" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D48" s="16">
         <v>2019</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F48" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G48" s="16" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="I48" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J48" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K48" s="16" t="s">
-        <v>449</v>
+        <v>428</v>
       </c>
       <c r="L48" s="16" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="M48" s="16" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="N48" s="16" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="49" spans="1:50" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D49" s="3">
         <v>2005</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>520</v>
+        <v>499</v>
       </c>
       <c r="I49" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>426</v>
+        <v>409</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N49" s="33" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:50" s="3" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D50" s="3">
         <v>2020</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>169</v>
+        <v>517</v>
       </c>
       <c r="I50" s="26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51" spans="1:50" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D51" s="16">
         <v>2011</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F51" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G51" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="I51" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J51" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K51" s="16" t="s">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="L51" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M51" s="16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="N51" s="18" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="O51" s="16" t="s">
-        <v>526</v>
+        <v>504</v>
       </c>
     </row>
     <row r="52" spans="1:50" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="24" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D52" s="3">
         <v>2003</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>518</v>
+        <v>497</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="I52" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M52" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:50" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A53" s="24" t="s">
-        <v>500</v>
+        <v>479</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>501</v>
+        <v>480</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>502</v>
+        <v>481</v>
       </c>
       <c r="D53" s="3">
         <v>2024</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>461</v>
+        <v>440</v>
       </c>
       <c r="F53" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
       <c r="I53" s="26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>505</v>
+        <v>484</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>506</v>
+        <v>485</v>
       </c>
       <c r="M53" s="3" t="s">
-        <v>503</v>
+        <v>482</v>
       </c>
       <c r="N53" s="3" t="s">
-        <v>507</v>
+        <v>486</v>
       </c>
       <c r="O53" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:50" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D54" s="16">
         <v>1995</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G54" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="H54" s="16" t="s">
-        <v>430</v>
+        <v>525</v>
       </c>
       <c r="I54" s="17" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="J54" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K54" s="16" t="s">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="L54" s="16" t="s">
-        <v>431</v>
+        <v>413</v>
       </c>
       <c r="M54" s="16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="N54" s="16" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="O54" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P54" s="19"/>
       <c r="Q54" s="19"/>
@@ -6834,178 +6832,178 @@
     </row>
     <row r="55" spans="1:50" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D55" s="3">
         <v>2023</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>432</v>
+        <v>414</v>
       </c>
       <c r="I55" s="26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>433</v>
+        <v>415</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="N55" s="3" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="O55" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:50" s="16" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D56" s="16">
         <v>2022</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F56" s="16" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G56" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="I56" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J56" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K56" s="16" t="s">
-        <v>434</v>
+        <v>416</v>
       </c>
       <c r="L56" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M56" s="16" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="N56" s="18" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="O56" s="16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="57" spans="1:50" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A57" s="24" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D57" s="3">
         <v>2018</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="I57" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K57" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M57" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="58" spans="1:50" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D58" s="4">
         <v>2002</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>523</v>
+        <v>508</v>
       </c>
       <c r="I58" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>435</v>
+        <v>417</v>
       </c>
       <c r="L58" s="4" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M58" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="N58" s="4" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="O58" s="4" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="P58" s="6"/>
       <c r="Q58" s="6"/>
@@ -7045,91 +7043,91 @@
     </row>
     <row r="59" spans="1:50" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D59" s="16">
         <v>2017</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F59" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G59" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="H59" s="16" t="s">
+        <v>526</v>
+      </c>
+      <c r="I59" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J59" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="K59" s="16" t="s">
+        <v>418</v>
+      </c>
+      <c r="L59" s="16" t="s">
+        <v>358</v>
+      </c>
+      <c r="M59" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G59" s="16" t="s">
-        <v>383</v>
-      </c>
-      <c r="H59" s="16" t="s">
-        <v>436</v>
-      </c>
-      <c r="I59" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="J59" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="K59" s="16" t="s">
-        <v>437</v>
-      </c>
-      <c r="L59" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="M59" s="16" t="s">
-        <v>13</v>
-      </c>
       <c r="N59" s="18" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="O59" s="16" t="s">
-        <v>527</v>
+        <v>505</v>
       </c>
     </row>
     <row r="60" spans="1:50" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A60" s="15" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D60" s="16">
         <v>2023</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F60" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="H60" s="16"/>
       <c r="I60" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J60" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K60" s="16" t="s">
-        <v>438</v>
+        <v>419</v>
       </c>
       <c r="L60" s="16" t="s">
-        <v>439</v>
+        <v>420</v>
       </c>
       <c r="M60" s="23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N60" s="18" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="P60" s="16"/>
       <c r="Q60" s="16"/>
@@ -7169,338 +7167,338 @@
     </row>
     <row r="61" spans="1:50" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D61" s="16">
         <v>2014</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F61" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G61" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="I61" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J61" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K61" s="16" t="s">
-        <v>440</v>
+        <v>421</v>
       </c>
       <c r="L61" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M61" s="16" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="N61" s="16" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="62" spans="1:50" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
-        <v>486</v>
+        <v>465</v>
       </c>
       <c r="B62" s="21" t="s">
-        <v>487</v>
+        <v>466</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>488</v>
+        <v>467</v>
       </c>
       <c r="D62" s="16">
         <v>2023</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>461</v>
+        <v>440</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>491</v>
+        <v>470</v>
       </c>
       <c r="G62" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="I62" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J62" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K62" s="16" t="s">
-        <v>493</v>
+        <v>472</v>
       </c>
       <c r="L62" s="16" t="s">
-        <v>492</v>
+        <v>471</v>
       </c>
       <c r="M62" s="16" t="s">
-        <v>489</v>
+        <v>468</v>
       </c>
       <c r="N62" s="16" t="s">
-        <v>490</v>
+        <v>469</v>
       </c>
     </row>
     <row r="63" spans="1:50" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A63" s="30" t="s">
-        <v>458</v>
+        <v>437</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>459</v>
+        <v>438</v>
       </c>
       <c r="C63" s="31" t="s">
-        <v>460</v>
+        <v>439</v>
       </c>
       <c r="D63" s="31">
         <v>2023</v>
       </c>
       <c r="E63" s="31" t="s">
-        <v>461</v>
+        <v>440</v>
       </c>
       <c r="F63" s="31" t="s">
-        <v>462</v>
+        <v>441</v>
       </c>
       <c r="G63" s="31" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>464</v>
+        <v>443</v>
       </c>
       <c r="I63" s="32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>465</v>
+        <v>444</v>
       </c>
       <c r="L63" s="31" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>463</v>
+        <v>442</v>
       </c>
       <c r="O63" s="31"/>
     </row>
     <row r="64" spans="1:50" s="16" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A64" s="15" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D64" s="16">
         <v>2022</v>
       </c>
       <c r="E64" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F64" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G64" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="I64" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J64" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K64" s="16" t="s">
-        <v>450</v>
+        <v>429</v>
       </c>
       <c r="L64" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M64" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N64" s="18" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="O64" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:50" s="16" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D65" s="16">
         <v>2021</v>
       </c>
       <c r="E65" s="16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F65" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G65" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="I65" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J65" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K65" s="16" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="L65" s="16" t="s">
-        <v>441</v>
+        <v>422</v>
       </c>
       <c r="M65" s="16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="N65" s="16" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="66" spans="1:50" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D66" s="16">
         <v>2011</v>
       </c>
       <c r="E66" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F66" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G66" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="I66" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J66" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K66" s="16" t="s">
-        <v>442</v>
+        <v>423</v>
       </c>
       <c r="L66" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M66" s="16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="N66" s="18" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="O66" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="67" spans="1:50" s="16" customFormat="1" ht="195" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D67" s="16">
         <v>2020</v>
       </c>
       <c r="E67" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F67" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G67" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="I67" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J67" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="K67" s="16" t="s">
+        <v>399</v>
+      </c>
+      <c r="L67" s="16" t="s">
+        <v>358</v>
+      </c>
+      <c r="M67" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="K67" s="16" t="s">
-        <v>413</v>
-      </c>
-      <c r="L67" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="M67" s="16" t="s">
-        <v>161</v>
-      </c>
       <c r="N67" s="16" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="O67" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="68" spans="1:50" s="29" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A68" s="24" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D68" s="3">
         <v>2023</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>519</v>
+        <v>498</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="H68" s="3"/>
       <c r="I68" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K68" s="3" t="s">
-        <v>443</v>
+        <v>424</v>
       </c>
       <c r="L68" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M68" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="N68" s="3"/>
       <c r="O68" s="3"/>
@@ -7542,84 +7540,84 @@
     </row>
     <row r="69" spans="1:50" s="16" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D69" s="16">
         <v>2020</v>
       </c>
       <c r="E69" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F69" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G69" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="H69" s="16" t="s">
-        <v>444</v>
+        <v>527</v>
       </c>
       <c r="I69" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J69" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K69" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L69" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M69" s="16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="N69" s="18" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="70" spans="1:50" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A70" s="24" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D70" s="3">
         <v>2018</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F70" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="I70" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="J70" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="K70" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="L70" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="M70" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="I70" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="J70" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="K70" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="L70" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="M70" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="P70" s="29"/>
       <c r="Q70" s="29"/>
@@ -7659,145 +7657,145 @@
     </row>
     <row r="71" spans="1:50" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A71" s="24" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D71" s="3">
         <v>2019</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F71" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="H71" s="27" t="s">
+        <v>518</v>
+      </c>
+      <c r="I71" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="J71" s="27" t="s">
+        <v>361</v>
+      </c>
+      <c r="K71" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="L71" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="M71" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G71" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="H71" s="27" t="s">
-        <v>445</v>
-      </c>
-      <c r="I71" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="J71" s="27" t="s">
-        <v>366</v>
-      </c>
-      <c r="K71" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="L71" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="M71" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="N71" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="72" spans="1:50" s="16" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A72" s="15" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D72" s="16">
         <v>2017</v>
       </c>
       <c r="E72" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F72" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G72" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="H72" s="16" t="s">
-        <v>78</v>
+        <v>528</v>
       </c>
       <c r="I72" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J72" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K72" s="16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="L72" s="16" t="s">
-        <v>446</v>
+        <v>425</v>
       </c>
       <c r="M72" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="N72" s="16" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="O72" s="16" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
-    <row r="73" spans="1:50" s="3" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:50" s="3" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A73" s="24" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B73" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D73" s="3">
         <v>1990</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>74</v>
+        <v>519</v>
       </c>
       <c r="I73" s="26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K73" s="3" t="s">
-        <v>447</v>
+        <v>426</v>
       </c>
       <c r="L73" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M73" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N73" s="3" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="O73" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:AX74">
-    <sortCondition ref="A2:A74"/>
+  <sortState ref="A2:O73">
+    <sortCondition ref="A2:A73"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
worked on OSf materials
</commit_message>
<xml_diff>
--- a/Opinion_paper/OSF/Literature_overview_72_publications.xlsx
+++ b/Opinion_paper/OSF/Literature_overview_72_publications.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20411"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5DE940-0E14-483C-9449-54D66743E086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3954A5F2-C74C-4364-A50B-8C62377156F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="529">
   <si>
     <t>Publication</t>
   </si>
@@ -681,9 +681,6 @@
     </r>
   </si>
   <si>
-    <t>review + empirical data</t>
-  </si>
-  <si>
     <t>differences between different speech synthesis methods</t>
   </si>
   <si>
@@ -1321,9 +1318,6 @@
     </r>
   </si>
   <si>
-    <t>empirical data, Eye tracking, fNIRS</t>
-  </si>
-  <si>
     <t>robot with gaze or a high human-like voice evoked more pleasure, higher, arousal, more perceived likability, and less negative attitudes; human-like voice evoked longer fixation duration; brain differences, but not correlated with ratings</t>
   </si>
   <si>
@@ -1433,9 +1427,6 @@
     <t>Despite variability between speakers, measures of mean F0, intensity range, articulation rate, average syllable duration, duration of final syllables, vocalic nucleus length of final unstressed syllables and pitch accent of final syllables emerged as possible acoustic variables contributing to within-speaker variations in speech naturalness</t>
   </si>
   <si>
-    <t>dysarthria</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Higgins, D., Zibrek, K., Cabral, J., Egan, D., &amp; McDonnell, R. (2022). Sympathy for the digital: Influence of synthetic voice on affinity, social presence and empathy for photorealistic virtual humans. </t>
     </r>
@@ -1496,10 +1487,6 @@
   </si>
   <si>
     <t>Abdulrahman, A., &amp; Richards, D. (2022). Is natural necessary? Human voice versus synthetic voice for intelligent virtual agents. Multimodal Technologies and Interaction, 6(7), 51.</t>
-  </si>
-  <si>
-    <t>"Participants in this study found
-the voice of the virtual advisor with TTS to be more eerie, but they rated both agents, with recorded voice and with TTS, similarly in terms of likeability. They further showed a similar attitude towards both agents in terms of co-presence and building trust."</t>
   </si>
   <si>
     <t>Euler, H. A., Merkel, A., Hente, K., Neef, N., von Gudenberg, A. W., &amp; Neumann, K. (2021). Speech restructuring group treatment for 6-to-9-year-old children who stutter: A therapeutic trial. Journal of Communication Disorders, 89, 106073.</t>
@@ -2466,9 +2453,6 @@
   </si>
   <si>
     <t>Nussbaum, C., Pöhlmann, M., Kreysa, H., &amp; Schweinberger, S. R. (2023). Perceived naturalness of emotional voice morphs. Cognition and Emotion, 1-17.</t>
-  </si>
-  <si>
-    <t>Morphey emotional voices</t>
   </si>
   <si>
     <t>voice morphing affects perceived naturalness, but is not correlated with emotional ratings</t>
@@ -2932,9 +2916,6 @@
     <t>human-likeness, artificiality, anthropomorphism</t>
   </si>
   <si>
-    <t xml:space="preserve">humanisation, human-likeness, anthropomorphism </t>
-  </si>
-  <si>
     <t>human-likeness, anthropomorphism, artificiality</t>
   </si>
   <si>
@@ -2979,9 +2960,6 @@
     <t>rating data + forced-choice pairwise comparison</t>
   </si>
   <si>
-    <t>(in)adequate prosody, anthropomorphism, human-likeness, aliveness</t>
-  </si>
-  <si>
     <t>anthropomorphism, human-likeness, acceptability</t>
   </si>
   <si>
@@ -2992,9 +2970,6 @@
   </si>
   <si>
     <t>voice quality, clarity</t>
-  </si>
-  <si>
-    <t>realism, human-likeness, robotic, anthropomorphism, expressiveness</t>
   </si>
   <si>
     <t>rating data + EMG</t>
@@ -3063,9 +3038,6 @@
     <t>voice-appearance matching task</t>
   </si>
   <si>
-    <t>speech quality, acceptability, acoustic abnormalities</t>
-  </si>
-  <si>
     <t>authenticity</t>
   </si>
   <si>
@@ -3096,27 +3068,12 @@
     <t>artificial, (dis)embodiment</t>
   </si>
   <si>
-    <t>memory performance</t>
-  </si>
-  <si>
     <t>artificial, robotic, human-likeness</t>
   </si>
   <si>
-    <t>review paper</t>
-  </si>
-  <si>
     <t>roboticness, monotony, human-likeness</t>
   </si>
   <si>
-    <t>dysarthria, severity</t>
-  </si>
-  <si>
-    <t>sorting method</t>
-  </si>
-  <si>
-    <t>dysarthria, bizarre</t>
-  </si>
-  <si>
     <t>human-likeness, anthropomorphism, machine-likeness, artificial, lifelike</t>
   </si>
   <si>
@@ -3129,12 +3086,6 @@
     <t>human-likeness, artificial</t>
   </si>
   <si>
-    <t>speech quality, acceptability, accentedness, (dis)fluency</t>
-  </si>
-  <si>
-    <t>realism, human-likeness,  organicness, animacy</t>
-  </si>
-  <si>
     <t>severity, acceptability, prosodic adequacy</t>
   </si>
   <si>
@@ -3198,9 +3149,6 @@
   </si>
   <si>
     <t>Schölderle</t>
-  </si>
-  <si>
-    <t>empirical data</t>
   </si>
   <si>
     <t>Childhood Dysarthria</t>
@@ -3326,9 +3274,6 @@
   </si>
   <si>
     <t>Amyotrophic lateral sclerosis (ALS)</t>
-  </si>
-  <si>
-    <t>empirical data and tool development</t>
   </si>
   <si>
     <t>voice banking, synthetic speech, speech-generating device, dysarthria, amyotrophic lateral sclerosis, intelligibility, naturalness, preference, attitude, statistical parametric speech synthesis, deep neural networks, unit-selection synthesis, waveform concatenation</t>
@@ -3739,6 +3684,63 @@
   </si>
   <si>
     <t>performance data, EEG data</t>
+  </si>
+  <si>
+    <t>rating data + tool development</t>
+  </si>
+  <si>
+    <t>forced-choice pairwise comparison + rating</t>
+  </si>
+  <si>
+    <t>Morphed emotional voices</t>
+  </si>
+  <si>
+    <t>rating data + performance data</t>
+  </si>
+  <si>
+    <t>memory performance, rating data, physiological response</t>
+  </si>
+  <si>
+    <t>literature review</t>
+  </si>
+  <si>
+    <t>rating data + conversation analysis</t>
+  </si>
+  <si>
+    <t>“How likely are you to hear a speaker like this, during a typical day?” (p 1541)</t>
+  </si>
+  <si>
+    <t>classification performance + sorting method</t>
+  </si>
+  <si>
+    <t>bizarre</t>
+  </si>
+  <si>
+    <t>severity</t>
+  </si>
+  <si>
+    <t>realism, human-likeness, organicness, animacy</t>
+  </si>
+  <si>
+    <t>realism, human-likeness, robotic, anthropomorphism</t>
+  </si>
+  <si>
+    <t>speech quality, acceptability, aberrant</t>
+  </si>
+  <si>
+    <t>speech quality, acceptability, accentedness, disfluency</t>
+  </si>
+  <si>
+    <t>prosodic adequacy, anthropomorphism, human-likeness, aliveness</t>
+  </si>
+  <si>
+    <t>Empirical data and tool development</t>
+  </si>
+  <si>
+    <t>Empirical data, Eye tracking, fNIRS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -4243,10 +4245,10 @@
   <dimension ref="A1:AX73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L20" sqref="L20"/>
+      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4269,13 +4271,13 @@
   <sheetData>
     <row r="1" spans="1:50" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>496</v>
+        <v>478</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>495</v>
+        <v>477</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>1</v>
@@ -4287,42 +4289,42 @@
         <v>2</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>432</v>
+        <v>416</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>497</v>
+        <v>479</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="M1" s="11" t="s">
         <v>3</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:50" s="14" customFormat="1" ht="204" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D2" s="14">
         <v>2022</v>
@@ -4334,36 +4336,36 @@
         <v>11</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>117</v>
+        <v>528</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:50" s="27" customFormat="1" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D3" s="27">
         <v>2021</v>
@@ -4375,22 +4377,22 @@
         <v>18</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>504</v>
+        <v>486</v>
       </c>
       <c r="I3" s="33" t="s">
         <v>8</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K3" s="34" t="s">
         <v>48</v>
       </c>
       <c r="L3" s="27" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="M3" s="27" t="s">
         <v>24</v>
@@ -4435,13 +4437,13 @@
     </row>
     <row r="4" spans="1:50" s="3" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D4" s="27">
         <v>2015</v>
@@ -4453,22 +4455,22 @@
         <v>18</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="H4" s="27" t="s">
-        <v>505</v>
+        <v>487</v>
       </c>
       <c r="I4" s="33" t="s">
         <v>8</v>
       </c>
       <c r="J4" s="27" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K4" s="27" t="s">
-        <v>498</v>
+        <v>480</v>
       </c>
       <c r="L4" s="27" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M4" s="27" t="s">
         <v>19</v>
@@ -4476,13 +4478,13 @@
     </row>
     <row r="5" spans="1:50" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D5" s="3">
         <v>2006</v>
@@ -4491,25 +4493,25 @@
         <v>51</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>525</v>
+        <v>507</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="I5" s="24" t="s">
         <v>13</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K5" s="25" t="s">
         <v>48</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>21</v>
@@ -4517,13 +4519,13 @@
     </row>
     <row r="6" spans="1:50" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D6" s="14">
         <v>2017</v>
@@ -4535,36 +4537,36 @@
         <v>11</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="I6" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7" spans="1:50" s="14" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D7" s="14">
         <v>2017</v>
@@ -4576,39 +4578,39 @@
         <v>11</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="I7" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>363</v>
+        <v>410</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M7" s="14" t="s">
         <v>27</v>
       </c>
       <c r="N7" s="16" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="O7" s="14" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="8" spans="1:50" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D8" s="14">
         <v>2018</v>
@@ -4620,42 +4622,42 @@
         <v>11</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>515</v>
+        <v>497</v>
       </c>
       <c r="I8" s="15" t="s">
         <v>8</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M8" s="14" t="s">
         <v>30</v>
       </c>
       <c r="N8" s="14" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="9" spans="1:50" s="17" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D9" s="14">
         <v>2018</v>
@@ -4667,20 +4669,20 @@
         <v>11</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M9" s="14" t="s">
         <v>27</v>
@@ -4725,13 +4727,13 @@
     </row>
     <row r="10" spans="1:50" s="4" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D10" s="4">
         <v>2017</v>
@@ -4743,36 +4745,36 @@
         <v>42</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>13</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>48</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:50" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D11" s="4">
         <v>2021</v>
@@ -4784,36 +4786,36 @@
         <v>11</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>13</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:50" s="17" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D12" s="14">
         <v>2017</v>
@@ -4825,26 +4827,26 @@
         <v>11</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="L12" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M12" s="14" t="s">
         <v>32</v>
       </c>
       <c r="N12" s="14" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="O12" s="14"/>
       <c r="P12" s="14"/>
@@ -4885,13 +4887,13 @@
     </row>
     <row r="13" spans="1:50" s="3" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D13" s="3">
         <v>2005</v>
@@ -4903,22 +4905,22 @@
         <v>34</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>506</v>
+        <v>488</v>
       </c>
       <c r="I13" s="24" t="s">
         <v>8</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M13" s="3" t="s">
         <v>35</v>
@@ -4926,13 +4928,13 @@
     </row>
     <row r="14" spans="1:50" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>482</v>
+        <v>464</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>483</v>
+        <v>465</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D14" s="4">
         <v>2024</v>
@@ -4941,76 +4943,76 @@
         <v>51</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>13</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>428</v>
+        <v>521</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="N14" s="36" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="O14" s="6"/>
     </row>
     <row r="15" spans="1:50" s="4" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D15" s="4">
         <v>2022</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>502</v>
+        <v>484</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>8</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>526</v>
+        <v>508</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
@@ -5050,40 +5052,40 @@
     </row>
     <row r="16" spans="1:50" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>442</v>
+        <v>425</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D16" s="4">
         <v>2024</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>484</v>
+        <v>466</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>13</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>527</v>
+        <v>509</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>443</v>
+        <v>426</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>444</v>
+        <v>427</v>
       </c>
       <c r="O16" s="4" t="s">
         <v>54</v>
@@ -5091,13 +5093,13 @@
     </row>
     <row r="17" spans="1:50" s="3" customFormat="1" ht="195" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D17" s="3">
         <v>2002</v>
@@ -5109,28 +5111,28 @@
         <v>52</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>507</v>
+        <v>489</v>
       </c>
       <c r="I17" s="24" t="s">
         <v>8</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M17" s="3" t="s">
         <v>55</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>501</v>
+        <v>483</v>
       </c>
       <c r="O17" s="3" t="s">
         <v>54</v>
@@ -5138,13 +5140,13 @@
     </row>
     <row r="18" spans="1:50" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D18" s="3">
         <v>2008</v>
@@ -5156,39 +5158,39 @@
         <v>52</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="I18" s="24" t="s">
         <v>8</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M18" s="3" t="s">
         <v>57</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:50" s="4" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D19" s="6">
         <v>2021</v>
@@ -5200,37 +5202,37 @@
         <v>42</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="37" t="s">
         <v>13</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>378</v>
+        <v>525</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="20" spans="1:50" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D20" s="3">
         <v>2021</v>
@@ -5239,39 +5241,39 @@
         <v>51</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="I20" s="24" t="s">
         <v>13</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K20" s="25" t="s">
         <v>48</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="21" spans="1:50" s="14" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D21" s="14">
         <v>2012</v>
@@ -5283,25 +5285,25 @@
         <v>42</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="I21" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K21" s="14" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="L21" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M21" s="14" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="N21" s="16" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="O21" s="14" t="s">
         <v>49</v>
@@ -5309,13 +5311,13 @@
     </row>
     <row r="22" spans="1:50" s="14" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D22" s="17">
         <v>2021</v>
@@ -5324,29 +5326,29 @@
         <v>51</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H22" s="17"/>
       <c r="I22" s="18" t="s">
         <v>13</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K22" s="17" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="L22" s="17" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M22" s="17" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="N22" s="16" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="O22" s="14" t="s">
         <v>49</v>
@@ -5389,13 +5391,13 @@
     </row>
     <row r="23" spans="1:50" s="14" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D23" s="14">
         <v>2007</v>
@@ -5407,36 +5409,36 @@
         <v>42</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>516</v>
+        <v>498</v>
       </c>
       <c r="I23" s="15" t="s">
         <v>8</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K23" s="14" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="L23" s="14" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="M23" s="14" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:50" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D24" s="3">
         <v>2016</v>
@@ -5445,36 +5447,36 @@
         <v>51</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>485</v>
+        <v>467</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="I24" s="24" t="s">
         <v>13</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:50" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D25" s="3">
         <v>2020</v>
@@ -5483,28 +5485,28 @@
         <v>51</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="I25" s="24" t="s">
         <v>13</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K25" s="25" t="s">
         <v>48</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="O25" s="3" t="s">
         <v>54</v>
@@ -5512,13 +5514,13 @@
     </row>
     <row r="26" spans="1:50" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D26" s="14">
         <v>2022</v>
@@ -5530,36 +5532,36 @@
         <v>42</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="I26" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K26" s="14" t="s">
-        <v>383</v>
+        <v>522</v>
       </c>
       <c r="L26" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M26" s="14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="N26" s="14" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="27" spans="1:50" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D27" s="14">
         <v>2021</v>
@@ -5571,75 +5573,75 @@
         <v>42</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>517</v>
+        <v>499</v>
       </c>
       <c r="I27" s="15" t="s">
         <v>8</v>
       </c>
       <c r="J27" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K27" s="14" t="s">
         <v>43</v>
       </c>
       <c r="L27" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M27" s="14" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="N27" s="16" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="O27" s="14" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="28" spans="1:50" s="14" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>445</v>
+        <v>428</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>446</v>
+        <v>429</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>447</v>
+        <v>430</v>
       </c>
       <c r="D28" s="14">
         <v>2024</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>449</v>
+        <v>526</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>448</v>
+        <v>431</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>451</v>
+        <v>433</v>
       </c>
       <c r="I28" s="15" t="s">
         <v>8</v>
       </c>
       <c r="J28" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K28" s="14" t="s">
         <v>26</v>
       </c>
       <c r="L28" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M28" s="14" t="s">
-        <v>452</v>
+        <v>434</v>
       </c>
       <c r="N28" s="14" t="s">
-        <v>450</v>
+        <v>432</v>
       </c>
       <c r="O28" s="14" t="s">
         <v>54</v>
@@ -5647,13 +5649,13 @@
     </row>
     <row r="29" spans="1:50" s="4" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D29" s="4">
         <v>2011</v>
@@ -5665,39 +5667,39 @@
         <v>42</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="I29" s="8" t="s">
         <v>13</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="M29" s="4" t="s">
         <v>59</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="O29" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:50" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B30" s="14" t="s">
         <v>60</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D30" s="14">
         <v>2013</v>
@@ -5709,25 +5711,25 @@
         <v>42</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="I30" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K30" s="14" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="L30" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M30" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N30" s="14" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="O30" s="14" t="s">
         <v>54</v>
@@ -5735,13 +5737,13 @@
     </row>
     <row r="31" spans="1:50" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D31" s="14">
         <v>2023</v>
@@ -5753,83 +5755,83 @@
         <v>42</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="I31" s="15" t="s">
         <v>8</v>
       </c>
       <c r="J31" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K31" s="14" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="L31" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M31" s="14" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="N31" s="16" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="32" spans="1:50" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
-        <v>453</v>
+        <v>435</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>454</v>
+        <v>436</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>455</v>
+        <v>437</v>
       </c>
       <c r="D32" s="3">
         <v>2019</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>436</v>
+        <v>51</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>486</v>
+        <v>468</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>457</v>
+        <v>439</v>
       </c>
       <c r="I32" s="24" t="s">
         <v>8</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>456</v>
+        <v>438</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>458</v>
+        <v>440</v>
       </c>
       <c r="N32" s="3" t="s">
-        <v>459</v>
+        <v>441</v>
       </c>
     </row>
     <row r="33" spans="1:15" s="4" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D33" s="4">
         <v>2022</v>
@@ -5838,42 +5840,42 @@
         <v>51</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>487</v>
+        <v>469</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="I33" s="8" t="s">
         <v>8</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="34" spans="1:15" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D34" s="3">
         <v>2015</v>
@@ -5885,42 +5887,42 @@
         <v>18</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="I34" s="24" t="s">
         <v>8</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="35" spans="1:15" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D35" s="3">
         <v>2016</v>
@@ -5929,45 +5931,45 @@
         <v>51</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>509</v>
+        <v>491</v>
       </c>
       <c r="I35" s="24" t="s">
         <v>8</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>430</v>
+        <v>414</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="N35" s="3" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="O35" s="3" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="36" spans="1:15" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B36" s="27" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D36" s="27">
         <v>2020</v>
@@ -5976,43 +5978,43 @@
         <v>6</v>
       </c>
       <c r="F36" s="27" t="s">
-        <v>488</v>
+        <v>470</v>
       </c>
       <c r="G36" s="27" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="H36" s="27" t="s">
-        <v>510</v>
+        <v>492</v>
       </c>
       <c r="I36" s="33" t="s">
         <v>8</v>
       </c>
       <c r="J36" s="27" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K36" s="27" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="L36" s="27" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="M36" s="27"/>
       <c r="N36" s="3" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="37" spans="1:15" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D37" s="14">
         <v>2023</v>
@@ -6021,39 +6023,39 @@
         <v>51</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>489</v>
+        <v>471</v>
       </c>
       <c r="G37" s="14" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="I37" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J37" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K37" s="14" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="L37" s="14" t="s">
-        <v>431</v>
+        <v>415</v>
       </c>
       <c r="M37" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N37" s="14" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="38" spans="1:15" s="14" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B38" s="14" t="s">
         <v>46</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D38" s="14">
         <v>2020</v>
@@ -6065,36 +6067,36 @@
         <v>42</v>
       </c>
       <c r="G38" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="I38" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J38" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K38" s="14" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
       <c r="L38" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M38" s="14" t="s">
         <v>47</v>
       </c>
       <c r="N38" s="16" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="39" spans="1:15" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D39" s="14">
         <v>2010</v>
@@ -6106,25 +6108,25 @@
         <v>42</v>
       </c>
       <c r="G39" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="I39" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J39" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K39" s="14" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="L39" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M39" s="14" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="N39" s="14" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="O39" s="14" t="s">
         <v>49</v>
@@ -6132,101 +6134,101 @@
     </row>
     <row r="40" spans="1:15" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
-        <v>468</v>
+        <v>450</v>
       </c>
       <c r="B40" s="32" t="s">
-        <v>469</v>
+        <v>451</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>470</v>
+        <v>452</v>
       </c>
       <c r="D40" s="3">
         <v>2022</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>436</v>
+        <v>51</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>471</v>
+        <v>453</v>
       </c>
       <c r="I40" s="24" t="s">
         <v>8</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>472</v>
+        <v>454</v>
       </c>
       <c r="N40" s="3" t="s">
-        <v>473</v>
+        <v>455</v>
       </c>
     </row>
     <row r="41" spans="1:15" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D41" s="14">
         <v>2023</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>102</v>
+        <v>527</v>
       </c>
       <c r="F41" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G41" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="I41" s="15" t="s">
         <v>8</v>
       </c>
       <c r="J41" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K41" s="14" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="L41" s="14" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="M41" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="N41" s="16" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="O41" s="14" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="42" spans="1:15" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B42" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>524</v>
+        <v>506</v>
       </c>
       <c r="D42" s="14">
         <v>2021</v>
@@ -6238,42 +6240,42 @@
         <v>15</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="H42" s="14" t="s">
-        <v>518</v>
+        <v>500</v>
       </c>
       <c r="I42" s="15" t="s">
         <v>8</v>
       </c>
       <c r="J42" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K42" s="14" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="L42" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M42" s="14" t="s">
         <v>16</v>
       </c>
       <c r="N42" s="14" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="O42" s="14" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="43" spans="1:15" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D43" s="3">
         <v>1997</v>
@@ -6282,86 +6284,86 @@
         <v>51</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>490</v>
+        <v>472</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="I43" s="24" t="s">
         <v>13</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>427</v>
+        <v>524</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M43" s="3" t="s">
         <v>62</v>
       </c>
       <c r="N43" s="3" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="44" spans="1:15" s="4" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D44" s="4">
         <v>2019</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="I44" s="8" t="s">
         <v>8</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="L44" s="4" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N44" s="4" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="45" spans="1:15" s="3" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D45" s="3">
         <v>1984</v>
@@ -6370,25 +6372,25 @@
         <v>51</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>511</v>
+        <v>493</v>
       </c>
       <c r="I45" s="24" t="s">
         <v>13</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M45" s="3" t="s">
         <v>64</v>
@@ -6396,13 +6398,13 @@
     </row>
     <row r="46" spans="1:15" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D46" s="14">
         <v>2022</v>
@@ -6411,42 +6413,42 @@
         <v>51</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>491</v>
+        <v>473</v>
       </c>
       <c r="G46" s="14" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="I46" s="15" t="s">
         <v>8</v>
       </c>
       <c r="J46" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K46" s="20" t="s">
         <v>48</v>
       </c>
       <c r="L46" s="14" t="s">
-        <v>355</v>
+        <v>510</v>
       </c>
       <c r="M46" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N46" s="14" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="47" spans="1:15" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D47" s="14">
         <v>2011</v>
@@ -6458,40 +6460,40 @@
         <v>42</v>
       </c>
       <c r="G47" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H47" s="14" t="s">
-        <v>519</v>
+        <v>501</v>
       </c>
       <c r="I47" s="15" t="s">
         <v>8</v>
       </c>
       <c r="J47" s="17" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K47" s="14" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="L47" s="14" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="M47" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N47" s="14" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="O47" s="17"/>
     </row>
     <row r="48" spans="1:15" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D48" s="14">
         <v>2019</v>
@@ -6503,36 +6505,36 @@
         <v>42</v>
       </c>
       <c r="G48" s="14" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="I48" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J48" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K48" s="14" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
       <c r="L48" s="14" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="M48" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N48" s="14" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="49" spans="1:50" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D49" s="3">
         <v>2005</v>
@@ -6541,45 +6543,45 @@
         <v>51</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>494</v>
+        <v>476</v>
       </c>
       <c r="I49" s="24" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>405</v>
+        <v>523</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>368</v>
+        <v>511</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N49" s="31" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:50" s="3" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D50" s="3">
         <v>2020</v>
@@ -6588,39 +6590,39 @@
         <v>51</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>512</v>
+        <v>494</v>
       </c>
       <c r="I50" s="24" t="s">
         <v>8</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:50" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D51" s="14">
         <v>2011</v>
@@ -6632,39 +6634,39 @@
         <v>42</v>
       </c>
       <c r="G51" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="I51" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J51" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K51" s="14" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="L51" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M51" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N51" s="16" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="O51" s="14" t="s">
-        <v>499</v>
+        <v>481</v>
       </c>
     </row>
     <row r="52" spans="1:50" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D52" s="3">
         <v>2003</v>
@@ -6673,69 +6675,69 @@
         <v>51</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>492</v>
+        <v>474</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="I52" s="24" t="s">
         <v>13</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K52" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="M52" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="L52" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="M52" s="3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:50" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A53" s="22" t="s">
-        <v>474</v>
+        <v>456</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>475</v>
+        <v>457</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>476</v>
+        <v>458</v>
       </c>
       <c r="D53" s="3">
         <v>2024</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>436</v>
+        <v>51</v>
       </c>
       <c r="F53" s="27" t="s">
         <v>18</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>478</v>
+        <v>460</v>
       </c>
       <c r="I53" s="24" t="s">
         <v>8</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>479</v>
+        <v>461</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>480</v>
+        <v>462</v>
       </c>
       <c r="M53" s="3" t="s">
-        <v>477</v>
+        <v>459</v>
       </c>
       <c r="N53" s="3" t="s">
-        <v>481</v>
+        <v>463</v>
       </c>
       <c r="O53" s="3" t="s">
         <v>54</v>
@@ -6743,13 +6745,13 @@
     </row>
     <row r="54" spans="1:50" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D54" s="14">
         <v>1995</v>
@@ -6761,28 +6763,28 @@
         <v>22</v>
       </c>
       <c r="G54" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H54" s="14" t="s">
-        <v>520</v>
+        <v>502</v>
       </c>
       <c r="I54" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J54" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K54" s="14" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="L54" s="14" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="M54" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N54" s="14" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="O54" s="14" t="s">
         <v>54</v>
@@ -6825,13 +6827,13 @@
     </row>
     <row r="55" spans="1:50" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D55" s="3">
         <v>2023</v>
@@ -6840,31 +6842,31 @@
         <v>51</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>224</v>
+        <v>512</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="I55" s="24" t="s">
         <v>8</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="N55" s="3" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="O55" s="3" t="s">
         <v>54</v>
@@ -6872,13 +6874,13 @@
     </row>
     <row r="56" spans="1:50" s="14" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D56" s="14">
         <v>2022</v>
@@ -6887,42 +6889,42 @@
         <v>51</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G56" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="I56" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J56" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K56" s="14" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L56" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M56" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N56" s="16" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="O56" s="14" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:50" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A57" s="22" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D57" s="3">
         <v>2018</v>
@@ -6934,33 +6936,33 @@
         <v>22</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="I57" s="24" t="s">
         <v>13</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K57" s="25" t="s">
         <v>48</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M57" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:50" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D58" s="4">
         <v>2002</v>
@@ -6969,34 +6971,34 @@
         <v>51</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>503</v>
+        <v>485</v>
       </c>
       <c r="I58" s="8" t="s">
         <v>13</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="L58" s="4" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M58" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="N58" s="4" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="O58" s="4" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="P58" s="6"/>
       <c r="Q58" s="6"/>
@@ -7036,13 +7038,13 @@
     </row>
     <row r="59" spans="1:50" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B59" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D59" s="14">
         <v>2017</v>
@@ -7054,42 +7056,42 @@
         <v>11</v>
       </c>
       <c r="G59" s="14" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="H59" s="14" t="s">
-        <v>521</v>
+        <v>503</v>
       </c>
       <c r="I59" s="15" t="s">
         <v>8</v>
       </c>
       <c r="J59" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K59" s="14" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="L59" s="14" t="s">
-        <v>355</v>
+        <v>513</v>
       </c>
       <c r="M59" s="14" t="s">
         <v>12</v>
       </c>
       <c r="N59" s="16" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="O59" s="14" t="s">
-        <v>500</v>
+        <v>482</v>
       </c>
     </row>
     <row r="60" spans="1:50" s="17" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B60" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D60" s="14">
         <v>2023</v>
@@ -7101,26 +7103,26 @@
         <v>11</v>
       </c>
       <c r="G60" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H60" s="14"/>
       <c r="I60" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J60" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K60" s="14" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="L60" s="14" t="s">
-        <v>416</v>
+        <v>514</v>
       </c>
       <c r="M60" s="21" t="s">
         <v>9</v>
       </c>
       <c r="N60" s="16" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="P60" s="14"/>
       <c r="Q60" s="14"/>
@@ -7160,13 +7162,13 @@
     </row>
     <row r="61" spans="1:50" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D61" s="14">
         <v>2014</v>
@@ -7178,119 +7180,119 @@
         <v>42</v>
       </c>
       <c r="G61" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="I61" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J61" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K61" s="14" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="L61" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M61" s="14" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="N61" s="14" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="62" spans="1:50" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
-        <v>460</v>
+        <v>442</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>461</v>
+        <v>443</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>462</v>
+        <v>444</v>
       </c>
       <c r="D62" s="14">
         <v>2023</v>
       </c>
       <c r="E62" s="14" t="s">
-        <v>436</v>
+        <v>51</v>
       </c>
       <c r="F62" s="14" t="s">
-        <v>465</v>
+        <v>447</v>
       </c>
       <c r="G62" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="I62" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J62" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K62" s="14" t="s">
-        <v>467</v>
+        <v>449</v>
       </c>
       <c r="L62" s="14" t="s">
-        <v>466</v>
+        <v>448</v>
       </c>
       <c r="M62" s="14" t="s">
-        <v>463</v>
+        <v>445</v>
       </c>
       <c r="N62" s="14" t="s">
-        <v>464</v>
+        <v>446</v>
       </c>
     </row>
     <row r="63" spans="1:50" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A63" s="28" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
       <c r="C63" s="29" t="s">
-        <v>435</v>
+        <v>419</v>
       </c>
       <c r="D63" s="29">
         <v>2023</v>
       </c>
       <c r="E63" s="29" t="s">
-        <v>436</v>
+        <v>51</v>
       </c>
       <c r="F63" s="29" t="s">
-        <v>437</v>
+        <v>420</v>
       </c>
       <c r="G63" s="29" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>439</v>
+        <v>422</v>
       </c>
       <c r="I63" s="30" t="s">
         <v>8</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>440</v>
+        <v>423</v>
       </c>
       <c r="L63" s="29" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>438</v>
+        <v>421</v>
       </c>
       <c r="O63" s="29"/>
     </row>
     <row r="64" spans="1:50" s="14" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B64" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D64" s="14">
         <v>2022</v>
@@ -7302,25 +7304,25 @@
         <v>42</v>
       </c>
       <c r="G64" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="I64" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J64" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K64" s="14" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
       <c r="L64" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M64" s="14" t="s">
         <v>45</v>
       </c>
       <c r="N64" s="16" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="O64" s="14" t="s">
         <v>49</v>
@@ -7328,54 +7330,54 @@
     </row>
     <row r="65" spans="1:50" s="14" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D65" s="14">
         <v>2021</v>
       </c>
       <c r="E65" s="14" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F65" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G65" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="I65" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J65" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K65" s="14" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="L65" s="14" t="s">
-        <v>418</v>
+        <v>515</v>
       </c>
       <c r="M65" s="14" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="N65" s="14" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="66" spans="1:50" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D66" s="14">
         <v>2011</v>
@@ -7387,25 +7389,25 @@
         <v>42</v>
       </c>
       <c r="G66" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="I66" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J66" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K66" s="14" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="L66" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M66" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N66" s="16" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="O66" s="14" t="s">
         <v>53</v>
@@ -7413,13 +7415,13 @@
     </row>
     <row r="67" spans="1:50" s="14" customFormat="1" ht="195" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D67" s="14">
         <v>2020</v>
@@ -7431,25 +7433,25 @@
         <v>42</v>
       </c>
       <c r="G67" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="I67" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J67" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K67" s="14" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="L67" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M67" s="14" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="N67" s="14" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="O67" s="14" t="s">
         <v>26</v>
@@ -7457,13 +7459,13 @@
     </row>
     <row r="68" spans="1:50" s="27" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A68" s="22" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D68" s="3">
         <v>2023</v>
@@ -7472,26 +7474,26 @@
         <v>51</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>493</v>
+        <v>475</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="H68" s="3"/>
       <c r="I68" s="24" t="s">
         <v>13</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K68" s="3" t="s">
-        <v>420</v>
+        <v>520</v>
       </c>
       <c r="L68" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M68" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N68" s="3"/>
       <c r="O68" s="3"/>
@@ -7533,13 +7535,13 @@
     </row>
     <row r="69" spans="1:50" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D69" s="14">
         <v>2020</v>
@@ -7551,39 +7553,39 @@
         <v>42</v>
       </c>
       <c r="G69" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H69" s="14" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I69" s="15" t="s">
         <v>8</v>
       </c>
       <c r="J69" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K69" s="14" t="s">
         <v>26</v>
       </c>
       <c r="L69" s="14" t="s">
-        <v>355</v>
+        <v>516</v>
       </c>
       <c r="M69" s="14" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="N69" s="16" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="70" spans="1:50" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A70" s="22" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D70" s="3">
         <v>2018</v>
@@ -7595,19 +7597,22 @@
         <v>40</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>370</v>
+        <v>364</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>517</v>
       </c>
       <c r="I70" s="24" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K70" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="L70" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M70" s="3" t="s">
         <v>41</v>
@@ -7650,13 +7655,13 @@
     </row>
     <row r="71" spans="1:50" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A71" s="22" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D71" s="3">
         <v>2019</v>
@@ -7668,39 +7673,36 @@
         <v>37</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="H71" s="25" t="s">
-        <v>513</v>
+        <v>495</v>
       </c>
       <c r="I71" s="26" t="s">
         <v>8</v>
       </c>
       <c r="J71" s="25" t="s">
-        <v>358</v>
-      </c>
-      <c r="K71" s="3" t="s">
-        <v>110</v>
+        <v>353</v>
       </c>
       <c r="L71" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M71" s="3" t="s">
         <v>38</v>
       </c>
       <c r="N71" s="3" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="72" spans="1:50" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D72" s="14">
         <v>2017</v>
@@ -7712,42 +7714,42 @@
         <v>42</v>
       </c>
       <c r="G72" s="14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H72" s="14" t="s">
-        <v>523</v>
+        <v>505</v>
       </c>
       <c r="I72" s="15" t="s">
         <v>8</v>
       </c>
       <c r="J72" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K72" s="14" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="L72" s="14" t="s">
-        <v>421</v>
+        <v>518</v>
       </c>
       <c r="M72" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N72" s="14" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="O72" s="14" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="73" spans="1:50" s="3" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A73" s="22" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B73" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D73" s="3">
         <v>1990</v>
@@ -7759,35 +7761,35 @@
         <v>37</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>514</v>
+        <v>496</v>
       </c>
       <c r="I73" s="24" t="s">
         <v>8</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="K73" s="3" t="s">
-        <v>422</v>
+        <v>519</v>
       </c>
       <c r="L73" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="M73" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N73" s="3" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="O73" s="3" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O73">
+  <sortState ref="A2:O73">
     <sortCondition ref="A2:A73"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
working on final tasks before submission
</commit_message>
<xml_diff>
--- a/Opinion_paper/OSF/Literature_overview_72_publications.xlsx
+++ b/Opinion_paper/OSF/Literature_overview_72_publications.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC34D2E-5504-4F3E-BB05-D7E9ACD51B29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7006E3E7-77E9-439D-B18B-BA1E48710E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="naturalness_publications" sheetId="1" r:id="rId1"/>
@@ -3841,7 +3841,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3950,9 +3950,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4237,31 +4234,31 @@
   <dimension ref="A1:AX73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L73" sqref="L73"/>
+      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="34.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" style="1" customWidth="1"/>
     <col min="6" max="7" width="24" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="9" customWidth="1"/>
-    <col min="10" max="10" width="21.140625" style="1" customWidth="1"/>
-    <col min="11" max="12" width="18.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="42.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="35.42578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="21.109375" style="1" customWidth="1"/>
+    <col min="11" max="12" width="18.5546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="42.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="35.44140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>429</v>
       </c>
@@ -4308,7 +4305,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="2" spans="1:50" s="14" customFormat="1" ht="204" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" s="14" customFormat="1" ht="204" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>183</v>
       </c>
@@ -4349,7 +4346,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="26" customFormat="1" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" s="26" customFormat="1" ht="168.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>189</v>
       </c>
@@ -4427,7 +4424,7 @@
       <c r="AW3" s="3"/>
       <c r="AX3" s="3"/>
     </row>
-    <row r="4" spans="1:50" s="3" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" s="3" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>208</v>
       </c>
@@ -4468,7 +4465,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:50" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
         <v>237</v>
       </c>
@@ -4509,7 +4506,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="6" spans="1:50" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>203</v>
       </c>
@@ -4550,7 +4547,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="7" spans="1:50" s="14" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" s="14" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>231</v>
       </c>
@@ -4594,7 +4591,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="8" spans="1:50" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>199</v>
       </c>
@@ -4641,7 +4638,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="9" spans="1:50" s="17" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" s="17" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>199</v>
       </c>
@@ -4717,7 +4714,7 @@
       <c r="AW9" s="14"/>
       <c r="AX9" s="14"/>
     </row>
-    <row r="10" spans="1:50" s="4" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" s="4" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>204</v>
       </c>
@@ -4758,7 +4755,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="11" spans="1:50" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" s="4" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>190</v>
       </c>
@@ -4799,7 +4796,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="12" spans="1:50" s="17" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" s="17" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>232</v>
       </c>
@@ -4877,7 +4874,7 @@
       <c r="AW12" s="14"/>
       <c r="AX12" s="14"/>
     </row>
-    <row r="13" spans="1:50" s="3" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" s="3" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
         <v>217</v>
       </c>
@@ -4918,7 +4915,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:50" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>415</v>
       </c>
@@ -4960,7 +4957,7 @@
       </c>
       <c r="O14" s="6"/>
     </row>
-    <row r="15" spans="1:50" s="4" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" s="4" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>184</v>
       </c>
@@ -5042,7 +5039,7 @@
       <c r="AW15" s="6"/>
       <c r="AX15" s="6"/>
     </row>
-    <row r="16" spans="1:50" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>379</v>
       </c>
@@ -5083,7 +5080,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:50" s="3" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:50" s="3" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
         <v>220</v>
       </c>
@@ -5130,7 +5127,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:50" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:50" s="3" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
         <v>216</v>
       </c>
@@ -5174,7 +5171,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="19" spans="1:50" s="4" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:50" s="4" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>225</v>
       </c>
@@ -5216,7 +5213,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="20" spans="1:50" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:50" s="3" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
         <v>191</v>
       </c>
@@ -5257,7 +5254,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="21" spans="1:50" s="14" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:50" s="14" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
         <v>235</v>
       </c>
@@ -5301,7 +5298,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:50" s="14" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:50" s="14" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
         <v>226</v>
       </c>
@@ -5381,7 +5378,7 @@
       <c r="AW22" s="17"/>
       <c r="AX22" s="17"/>
     </row>
-    <row r="23" spans="1:50" s="14" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:50" s="14" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
         <v>215</v>
       </c>
@@ -5422,7 +5419,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="24" spans="1:50" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:50" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A24" s="21" t="s">
         <v>207</v>
       </c>
@@ -5460,7 +5457,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:50" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:50" s="3" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A25" s="21" t="s">
         <v>195</v>
       </c>
@@ -5504,7 +5501,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:50" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:50" s="14" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
         <v>185</v>
       </c>
@@ -5545,7 +5542,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="27" spans="1:50" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:50" s="14" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
         <v>192</v>
       </c>
@@ -5592,7 +5589,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="28" spans="1:50" s="14" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:50" s="14" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
         <v>382</v>
       </c>
@@ -5639,7 +5636,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:50" s="4" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:50" s="4" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>236</v>
       </c>
@@ -5683,7 +5680,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:50" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:50" s="14" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>210</v>
       </c>
@@ -5727,7 +5724,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:50" s="14" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:50" s="14" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
         <v>178</v>
       </c>
@@ -5771,7 +5768,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="32" spans="1:50" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:50" s="3" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A32" s="21" t="s">
         <v>388</v>
       </c>
@@ -5815,7 +5812,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="33" spans="1:15" s="4" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" s="4" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>186</v>
       </c>
@@ -5859,7 +5856,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="34" spans="1:15" s="3" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A34" s="21" t="s">
         <v>209</v>
       </c>
@@ -5906,7 +5903,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="35" spans="1:15" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
         <v>233</v>
       </c>
@@ -5953,7 +5950,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" s="3" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A36" s="21" t="s">
         <v>196</v>
       </c>
@@ -6000,7 +5997,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" s="14" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
         <v>179</v>
       </c>
@@ -6041,7 +6038,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" s="14" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
         <v>197</v>
       </c>
@@ -6082,7 +6079,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="39" spans="1:15" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
         <v>214</v>
       </c>
@@ -6126,7 +6123,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:15" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" s="3" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A40" s="21" t="s">
         <v>402</v>
       </c>
@@ -6167,7 +6164,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="41" spans="1:15" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" s="14" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
         <v>180</v>
       </c>
@@ -6214,7 +6211,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="42" spans="1:15" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
         <v>193</v>
       </c>
@@ -6261,7 +6258,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="43" spans="1:15" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" s="3" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A43" s="21" t="s">
         <v>221</v>
       </c>
@@ -6305,7 +6302,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="44" spans="1:15" s="4" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" s="4" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>229</v>
       </c>
@@ -6349,7 +6346,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="45" spans="1:15" s="3" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A45" s="21" t="s">
         <v>223</v>
       </c>
@@ -6390,7 +6387,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="46" spans="1:15" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" s="14" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
         <v>187</v>
       </c>
@@ -6434,7 +6431,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="47" spans="1:15" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" s="14" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>211</v>
       </c>
@@ -6479,7 +6476,7 @@
       </c>
       <c r="O47" s="17"/>
     </row>
-    <row r="48" spans="1:15" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" s="14" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
         <v>230</v>
       </c>
@@ -6520,7 +6517,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="49" spans="1:50" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:50" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A49" s="21" t="s">
         <v>218</v>
       </c>
@@ -6567,7 +6564,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="50" spans="1:50" s="3" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:50" s="3" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A50" s="21" t="s">
         <v>198</v>
       </c>
@@ -6608,7 +6605,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="51" spans="1:50" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:50" s="14" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
         <v>212</v>
       </c>
@@ -6652,7 +6649,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="52" spans="1:50" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:50" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A52" s="21" t="s">
         <v>219</v>
       </c>
@@ -6690,7 +6687,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:50" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:50" s="3" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A53" s="21" t="s">
         <v>408</v>
       </c>
@@ -6737,7 +6734,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:50" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:50" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A54" s="13" t="s">
         <v>239</v>
       </c>
@@ -6819,7 +6816,7 @@
       <c r="AW54" s="17"/>
       <c r="AX54" s="17"/>
     </row>
-    <row r="55" spans="1:50" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:50" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A55" s="21" t="s">
         <v>181</v>
       </c>
@@ -6866,7 +6863,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:50" s="14" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:50" s="14" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A56" s="13" t="s">
         <v>224</v>
       </c>
@@ -6910,7 +6907,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="1:50" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:50" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A57" s="21" t="s">
         <v>200</v>
       </c>
@@ -6948,7 +6945,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="58" spans="1:50" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:50" s="4" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>238</v>
       </c>
@@ -7030,7 +7027,7 @@
       <c r="AW58" s="6"/>
       <c r="AX58" s="6"/>
     </row>
-    <row r="59" spans="1:50" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:50" s="14" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
         <v>205</v>
       </c>
@@ -7077,7 +7074,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="60" spans="1:50" s="17" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:50" s="17" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A60" s="13" t="s">
         <v>182</v>
       </c>
@@ -7112,7 +7109,7 @@
       <c r="L60" s="14" t="s">
         <v>465</v>
       </c>
-      <c r="M60" s="37" t="s">
+      <c r="M60" s="14" t="s">
         <v>517</v>
       </c>
       <c r="N60" s="16" t="s">
@@ -7154,7 +7151,7 @@
       <c r="AW60" s="14"/>
       <c r="AX60" s="14"/>
     </row>
-    <row r="61" spans="1:50" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:50" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A61" s="13" t="s">
         <v>234</v>
       </c>
@@ -7195,7 +7192,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="62" spans="1:50" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:50" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
         <v>395</v>
       </c>
@@ -7236,7 +7233,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="63" spans="1:50" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:50" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A63" s="27" t="s">
         <v>373</v>
       </c>
@@ -7278,7 +7275,7 @@
       </c>
       <c r="O63" s="28"/>
     </row>
-    <row r="64" spans="1:50" s="14" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:50" s="14" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
         <v>188</v>
       </c>
@@ -7322,7 +7319,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="65" spans="1:50" s="14" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:50" s="14" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
         <v>194</v>
       </c>
@@ -7363,7 +7360,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="66" spans="1:50" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:50" s="14" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
         <v>213</v>
       </c>
@@ -7407,7 +7404,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="67" spans="1:50" s="14" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:50" s="14" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
         <v>227</v>
       </c>
@@ -7451,7 +7448,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="1:50" s="26" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:50" s="26" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A68" s="21" t="s">
         <v>240</v>
       </c>
@@ -7527,7 +7524,7 @@
       <c r="AW68" s="3"/>
       <c r="AX68" s="3"/>
     </row>
-    <row r="69" spans="1:50" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:50" s="14" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
         <v>228</v>
       </c>
@@ -7571,7 +7568,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="70" spans="1:50" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:50" s="3" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A70" s="21" t="s">
         <v>201</v>
       </c>
@@ -7647,7 +7644,7 @@
       <c r="AW70" s="26"/>
       <c r="AX70" s="26"/>
     </row>
-    <row r="71" spans="1:50" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:50" s="3" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A71" s="21" t="s">
         <v>202</v>
       </c>
@@ -7688,7 +7685,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="72" spans="1:50" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:50" s="14" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A72" s="13" t="s">
         <v>206</v>
       </c>
@@ -7735,7 +7732,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="73" spans="1:50" s="3" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:50" s="3" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A73" s="21" t="s">
         <v>222</v>
       </c>
@@ -7783,7 +7780,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:O73">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O73">
     <sortCondition ref="A2:A73"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
revision of definitions on OSF
</commit_message>
<xml_diff>
--- a/Opinion_paper/OSF/Literature_overview_72_publications.xlsx
+++ b/Opinion_paper/OSF/Literature_overview_72_publications.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E550F366-26F5-421D-A421-89D147EB8984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0EDDA4-4BBA-4585-B010-46E5A197C688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4245,10 +4245,10 @@
   <dimension ref="A1:AX73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L49" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M52" sqref="M52"/>
+      <selection pane="bottomRight" activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6827,50 +6827,50 @@
       <c r="AW54" s="17"/>
       <c r="AX54" s="17"/>
     </row>
-    <row r="55" spans="1:50" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A55" s="21" t="s">
+    <row r="55" spans="1:50" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D55" s="4">
         <v>2023</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E55" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="F55" s="4" t="s">
         <v>463</v>
       </c>
-      <c r="G55" s="3" t="s">
+      <c r="G55" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="H55" s="3" t="s">
+      <c r="H55" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="I55" s="23" t="s">
+      <c r="I55" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J55" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="K55" s="3" t="s">
+      <c r="J55" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="K55" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="L55" s="3" t="s">
+      <c r="L55" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="M55" s="3" t="s">
+      <c r="M55" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="N55" s="3" t="s">
+      <c r="N55" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="O55" s="3" t="s">
+      <c r="O55" s="4" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
status sent to coauthors
</commit_message>
<xml_diff>
--- a/Opinion_paper/OSF/Literature_overview_72_publications.xlsx
+++ b/Opinion_paper/OSF/Literature_overview_72_publications.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0EDDA4-4BBA-4585-B010-46E5A197C688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977BA45B-FB6D-429C-AB42-7AE96CAAACB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4245,10 +4245,10 @@
   <dimension ref="A1:AX73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B70" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F56" sqref="F56"/>
+      <selection pane="bottomRight" activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>